<commit_message>
ontology avec Google Refine ok :+1:
</commit_message>
<xml_diff>
--- a/LotR.xlsx
+++ b/LotR.xlsx
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="W6" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X6" s="9">
         <v>3</v>

</xml_diff>